<commit_message>
Se anexa la matriz de riesgos actualizada con riesgos asociados a los servicios SOAP
</commit_message>
<xml_diff>
--- a/Matriz_riesgos-C1-2023-QA-Calidad-RF.xlsx
+++ b/Matriz_riesgos-C1-2023-QA-Calidad-RF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\IdeaProjects\sofka\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31910593-B8C3-44FB-ACFF-C0CF2D277427}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82485F8-83C9-4848-B392-AEEE6545155E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{FE293536-0AB4-4C90-BA1D-969299BE5294}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="132">
   <si>
     <t>Consecutivo</t>
   </si>
@@ -428,6 +428,12 @@
   </si>
   <si>
     <t>Asignar responsabilidades claras en el equipo asociadas a la aprobación de los gastos, asignación de recursos financieros y realización de los pagos correspondientes</t>
+  </si>
+  <si>
+    <t>la posibilidad de recibir respuestas erroneas de los servicios SOAP cuando el usuario ingresa datos de entrada válidos</t>
+  </si>
+  <si>
+    <t>Posibilidad de recibir respuestas erroneas de los servicios SOAP cuando el usuario ingresa datos de entrada invalidos</t>
   </si>
 </sst>
 </file>
@@ -602,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -667,6 +673,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -675,11 +682,47 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="56">
+    <dxf>
+      <font>
+        <color rgb="FF92D050"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFFFF00"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1015,39 +1058,6 @@
     </dxf>
     <dxf>
       <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF92D050"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF92D050"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1411,20 +1421,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0A2D8B7-11B6-4C9F-8DFB-809F67662B71}" name="Table_111" displayName="Table_111" ref="A7:L37" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E0A2D8B7-11B6-4C9F-8DFB-809F67662B71}" name="Table_111" displayName="Table_111" ref="A7:L39" headerRowDxfId="28">
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B4D1C6A1-B542-4FD4-A89E-03554F558036}" name="Consecutivo" dataDxfId="24"/>
-    <tableColumn id="2" xr3:uid="{20B67D71-1860-424A-9D54-272F92E857F2}" name="Descripción Riesgo" dataDxfId="23"/>
-    <tableColumn id="3" xr3:uid="{99024EC6-96A7-43F7-A843-1739760F5E00}" name="Tipo de Riesgo" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{AFBD5C4C-03B7-4915-81C8-DA03F79459FC}" name="Probabilidad de ocurrencia" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{D5BD74D4-B032-4267-8476-E8189742EFF9}" name="Impacto" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{C40EBB4C-64E3-4329-ACC5-BB89D2E27445}" name="Riesgo" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{4F119BEE-18FA-47FA-88FB-21ED334053FD}" name="Riesgo " dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{3FDDB74E-AF6B-4B35-81C7-640CD8656687}" name="Acción" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{7DA0AD36-AACB-49C6-97E7-9F41DC268BA1}" name="Plan de Acción" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{10D58CD4-A65C-4CE8-87A7-FA74ABFF1C93}" name="Responsable de la Acción" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{FD926A79-4873-4A99-89A9-E351E2B78025}" name="Fecha Compromiso " dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{F55FD157-6FFF-497B-8F3D-C4A8F1183083}" name="Estado" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{B4D1C6A1-B542-4FD4-A89E-03554F558036}" name="Consecutivo" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{20B67D71-1860-424A-9D54-272F92E857F2}" name="Descripción Riesgo" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{99024EC6-96A7-43F7-A843-1739760F5E00}" name="Tipo de Riesgo" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{AFBD5C4C-03B7-4915-81C8-DA03F79459FC}" name="Probabilidad de ocurrencia" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{D5BD74D4-B032-4267-8476-E8189742EFF9}" name="Impacto" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{C40EBB4C-64E3-4329-ACC5-BB89D2E27445}" name="Riesgo" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{4F119BEE-18FA-47FA-88FB-21ED334053FD}" name="Riesgo " dataDxfId="21"/>
+    <tableColumn id="9" xr3:uid="{3FDDB74E-AF6B-4B35-81C7-640CD8656687}" name="Acción" dataDxfId="20"/>
+    <tableColumn id="10" xr3:uid="{7DA0AD36-AACB-49C6-97E7-9F41DC268BA1}" name="Plan de Acción" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{10D58CD4-A65C-4CE8-87A7-FA74ABFF1C93}" name="Responsable de la Acción" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{FD926A79-4873-4A99-89A9-E351E2B78025}" name="Fecha Compromiso " dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{F55FD157-6FFF-497B-8F3D-C4A8F1183083}" name="Estado" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Matriz de Riesgo-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1433,8 +1443,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F99F682-9124-4141-9886-84FF3DF70E95}" name="Table_2" displayName="Table_2" ref="A1:B5">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6FCFD6CF-D05E-47EA-A6EC-3BAF9E14DCAE}" name="Plan de Acción" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{78FB452F-ECA1-475A-8C9B-B9544E7D6DDC}" name="Descripción" dataDxfId="11"/>
+    <tableColumn id="1" xr3:uid="{6FCFD6CF-D05E-47EA-A6EC-3BAF9E14DCAE}" name="Plan de Acción" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{78FB452F-ECA1-475A-8C9B-B9544E7D6DDC}" name="Descripción" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1443,7 +1453,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5B45C15-A36D-4BC0-9E74-AFD731CE3381}" name="Table_3" displayName="Table_3" ref="D1:D3">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C85C2E5D-B09A-4D5F-97C0-AB5A81FEEB2A}" name="Tipo de Riesg" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{C85C2E5D-B09A-4D5F-97C0-AB5A81FEEB2A}" name="Tipo de Riesg" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1452,9 +1462,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7C4D1B14-5B86-4DBF-94FE-8B73D66225C7}" name="Table_4" displayName="Table_4" ref="F1:H6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CEC6DF00-0D9C-4327-B944-A9256E007FF6}" name="Probabilidad" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4BF8DB27-E23F-4A92-A495-BB5C0F6632A5}" name="Evaluación" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{21A83028-31E0-46BC-BB5A-34C6ECAFEDD3}" name="Definición" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{CEC6DF00-0D9C-4327-B944-A9256E007FF6}" name="Probabilidad" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{4BF8DB27-E23F-4A92-A495-BB5C0F6632A5}" name="Evaluación" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{21A83028-31E0-46BC-BB5A-34C6ECAFEDD3}" name="Definición" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1463,9 +1473,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FDE817A5-0B61-430E-9F87-9AF8174F3EF9}" name="Table_5" displayName="Table_5" ref="J1:L6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{63F79449-20E3-4F6D-B5D3-4F3DF0AB1417}" name="Impacto" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{351FFBC1-5848-4E2F-A294-8C5D1675AFA7}" name="Evaluación" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{9BC32A01-D298-4AC4-A8E3-59607DC50617}" name="Definición" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{63F79449-20E3-4F6D-B5D3-4F3DF0AB1417}" name="Impacto" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{351FFBC1-5848-4E2F-A294-8C5D1675AFA7}" name="Evaluación" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{9BC32A01-D298-4AC4-A8E3-59607DC50617}" name="Definición" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1474,7 +1484,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E9C38933-B1EC-4CE4-82B2-485B6835F881}" name="Table_6" displayName="Table_6" ref="A8:A10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A4F5C3B6-7FFF-4B5A-AD9D-721C7A161134}" name="Responsable Calidad" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{A4F5C3B6-7FFF-4B5A-AD9D-721C7A161134}" name="Responsable Calidad" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1483,7 +1493,7 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{27D1D1C5-CBC3-454D-9B03-68A1FB92038C}" name="Table_7" displayName="Table_7" ref="D8:D10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{61089E2C-4840-4002-A9EA-E876FAFC254E}" name="Plan de Calidad" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{61089E2C-4840-4002-A9EA-E876FAFC254E}" name="Plan de Calidad" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1492,7 +1502,7 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E9CFF31-25F5-4F31-8D7A-71C8788590E5}" name="Table_8" displayName="Table_8" ref="F8:F10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{718A55F6-D7C9-4551-AF65-357BA4E12B01}" name="Historia de Usuario" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{718A55F6-D7C9-4551-AF65-357BA4E12B01}" name="Historia de Usuario" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1501,7 +1511,7 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1D77D549-EA02-4FB7-B0E5-946DBD6CA201}" name="Table_9" displayName="Table_9" ref="A12:A14">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B6AE7DE1-B7F0-4FA4-939E-3F45CBF4E99A}" name="Estado" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B6AE7DE1-B7F0-4FA4-939E-3F45CBF4E99A}" name="Estado" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1806,8 +1816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7AC659-34BE-478B-80F3-AAD59B518E91}">
   <dimension ref="A1:L1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" workbookViewId="0">
-      <selection activeCell="I35" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1829,88 +1839,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="28"/>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
     </row>
     <row r="2" spans="1:12" ht="15" customHeight="1">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="A2" s="30"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="30"/>
+      <c r="L2" s="30"/>
     </row>
     <row r="3" spans="1:12" ht="15" customHeight="1">
-      <c r="A3" s="29"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
+      <c r="A3" s="30"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="30"/>
+      <c r="L3" s="30"/>
     </row>
     <row r="4" spans="1:12" ht="15" customHeight="1">
-      <c r="A4" s="29"/>
-      <c r="B4" s="29"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
     </row>
     <row r="5" spans="1:12" ht="15" customHeight="1">
-      <c r="A5" s="29"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="29"/>
-      <c r="K5" s="29"/>
-      <c r="L5" s="29"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
     </row>
     <row r="6" spans="1:12" ht="15" customHeight="1">
-      <c r="A6" s="29"/>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="29"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="30"/>
+      <c r="L6" s="30"/>
     </row>
     <row r="7" spans="1:12" s="11" customFormat="1" ht="27" customHeight="1">
       <c r="A7" s="2" t="s">
@@ -3063,101 +3073,149 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1">
-      <c r="I38" s="6"/>
-    </row>
-    <row r="39" spans="1:12" ht="15.75" customHeight="1">
-      <c r="I39" s="6"/>
+    <row r="38" spans="1:12" ht="30">
+      <c r="A38" s="8">
+        <v>31</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="8">
+        <v>4</v>
+      </c>
+      <c r="E38" s="8">
+        <v>5</v>
+      </c>
+      <c r="F38" s="28"/>
+      <c r="G38" s="7">
+        <f xml:space="preserve"> Table_111[[#This Row],[Probabilidad de ocurrencia]]*Table_111[[#This Row],[Impacto]]</f>
+        <v>20</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I38" s="10"/>
+      <c r="J38" s="28"/>
+    </row>
+    <row r="39" spans="1:12" ht="30">
+      <c r="A39" s="33">
+        <v>32</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="8">
+        <v>4</v>
+      </c>
+      <c r="E39" s="8">
+        <v>5</v>
+      </c>
+      <c r="F39" s="28"/>
+      <c r="G39" s="7">
+        <f xml:space="preserve"> Table_111[[#This Row],[Probabilidad de ocurrencia]]*Table_111[[#This Row],[Impacto]]</f>
+        <v>20</v>
+      </c>
+      <c r="H39" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="10"/>
+      <c r="J39" s="28"/>
     </row>
     <row r="40" spans="1:12" ht="15.75" customHeight="1">
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B41" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="31"/>
+    <row r="41" spans="1:12" ht="15.75" customHeight="1">
       <c r="I41" s="6"/>
     </row>
     <row r="42" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B42" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C42" s="13"/>
       <c r="I42" s="6"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" customHeight="1">
-      <c r="B43" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C43" s="15"/>
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
-      <c r="B44" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="17"/>
+    <row r="44" spans="1:12" ht="15.75" customHeight="1">
       <c r="I44" s="6"/>
     </row>
     <row r="45" spans="1:12" ht="15.75" customHeight="1">
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1">
+    <row r="46" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B46" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="32"/>
       <c r="I46" s="6"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" customHeight="1">
+      <c r="B47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C47" s="13"/>
       <c r="I47" s="6"/>
     </row>
     <row r="48" spans="1:12" ht="15.75" customHeight="1">
+      <c r="B48" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="15"/>
       <c r="I48" s="6"/>
     </row>
-    <row r="49" spans="9:9" ht="15.75" customHeight="1">
+    <row r="49" spans="2:9" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B49" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C49" s="17"/>
       <c r="I49" s="6"/>
     </row>
-    <row r="50" spans="9:9" ht="15.75" customHeight="1">
+    <row r="50" spans="2:9" ht="15.75" customHeight="1">
       <c r="I50" s="6"/>
     </row>
-    <row r="51" spans="9:9" ht="15.75" customHeight="1">
+    <row r="51" spans="2:9" ht="15.75" customHeight="1">
       <c r="I51" s="6"/>
     </row>
-    <row r="52" spans="9:9" ht="15.75" customHeight="1">
+    <row r="52" spans="2:9" ht="15.75" customHeight="1">
       <c r="I52" s="6"/>
     </row>
-    <row r="53" spans="9:9" ht="15.75" customHeight="1">
+    <row r="53" spans="2:9" ht="15.75" customHeight="1">
       <c r="I53" s="6"/>
     </row>
-    <row r="54" spans="9:9" ht="15.75" customHeight="1">
+    <row r="54" spans="2:9" ht="15.75" customHeight="1">
       <c r="I54" s="6"/>
     </row>
-    <row r="55" spans="9:9" ht="15.75" customHeight="1">
+    <row r="55" spans="2:9" ht="15.75" customHeight="1">
       <c r="I55" s="6"/>
     </row>
-    <row r="56" spans="9:9" ht="15.75" customHeight="1">
+    <row r="56" spans="2:9" ht="15.75" customHeight="1">
       <c r="I56" s="6"/>
     </row>
-    <row r="57" spans="9:9" ht="15.75" customHeight="1">
+    <row r="57" spans="2:9" ht="15.75" customHeight="1">
       <c r="I57" s="6"/>
     </row>
-    <row r="58" spans="9:9" ht="15.75" customHeight="1">
+    <row r="58" spans="2:9" ht="15.75" customHeight="1">
       <c r="I58" s="6"/>
     </row>
-    <row r="59" spans="9:9" ht="15.75" customHeight="1">
+    <row r="59" spans="2:9" ht="15.75" customHeight="1">
       <c r="I59" s="6"/>
     </row>
-    <row r="60" spans="9:9" ht="15.75" customHeight="1">
+    <row r="60" spans="2:9" ht="15.75" customHeight="1">
       <c r="I60" s="6"/>
     </row>
-    <row r="61" spans="9:9" ht="15.75" customHeight="1">
+    <row r="61" spans="2:9" ht="15.75" customHeight="1">
       <c r="I61" s="6"/>
     </row>
-    <row r="62" spans="9:9" ht="15.75" customHeight="1">
+    <row r="62" spans="2:9" ht="15.75" customHeight="1">
       <c r="I62" s="6"/>
     </row>
-    <row r="63" spans="9:9" ht="15.75" customHeight="1">
+    <row r="63" spans="2:9" ht="15.75" customHeight="1">
       <c r="I63" s="6"/>
     </row>
-    <row r="64" spans="9:9" ht="15.75" customHeight="1">
+    <row r="64" spans="2:9" ht="15.75" customHeight="1">
       <c r="I64" s="6"/>
     </row>
     <row r="65" spans="9:9" ht="15.75" customHeight="1">
@@ -5998,18 +6056,18 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:L6"/>
-    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B46:C46"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G1009">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>20</formula>
       <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>11</formula>
       <formula>19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>
@@ -6078,10 +6136,10 @@
       <c r="L1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="N1" s="30" t="s">
+      <c r="N1" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="31"/>
+      <c r="O1" s="32"/>
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="7" t="s">

</xml_diff>

<commit_message>
Se eliminan los responsables de la acción de mitigación de cada riesgo
</commit_message>
<xml_diff>
--- a/Matriz_riesgos-C1-2023-QA-Calidad-RF.xlsx
+++ b/Matriz_riesgos-C1-2023-QA-Calidad-RF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DISENO11\IdeaProjects\sofka\C1-2023-QA-Calidad-RF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82485F8-83C9-4848-B392-AEEE6545155E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E3E7B7D-AF9F-418B-A228-1DE864517AEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{FE293536-0AB4-4C90-BA1D-969299BE5294}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="126">
   <si>
     <t>Consecutivo</t>
   </si>
@@ -297,16 +297,9 @@
     <t>Problemas de falta de soporte técnico y mantenimiento que puedan afectar la capacidad del sistema para adaptarse a cambios en la industria en las necesidades del negocio</t>
   </si>
   <si>
-    <t xml:space="preserve">QA
-</t>
-  </si>
-  <si>
     <t>Establecer acuerdos de nivel de servicio con proveedores externos para minimizar el riesgo de fallos en la integración con sistemas externos</t>
   </si>
   <si>
-    <t>PO</t>
-  </si>
-  <si>
     <t>Se recomienda incorporar pruebas de usabilidad en otras etapas del proyecto para validar que los mensajes de error y confirmación sean claros para el cliente</t>
   </si>
   <si>
@@ -316,29 +309,15 @@
     <t>Realizar copias de seguridad frecuentes y tener un plan de recuperación en caso de pérdida de información</t>
   </si>
   <si>
-    <t>PO
-Equipo desarrollo</t>
-  </si>
-  <si>
     <t>Se recomienda utilizar servicios de traducción y conversión de moneda para adaptar la página web a los clientes extranjeros</t>
   </si>
   <si>
-    <t>Scrum Master</t>
-  </si>
-  <si>
     <t>Se recomienda realizar auditorias internas de seguridad para identificar posibles vulnerabilidades en la página web y los sistemas de almacenamiento de datos</t>
   </si>
   <si>
-    <t>Experto seguridad de la información
-Equipo desarrollo</t>
-  </si>
-  <si>
     <t>Se recomienda la realización de pruebas de carga para determinar la capacidad de la página web para manejar un gran número de solicitudes y usuarios concurrentes</t>
   </si>
   <si>
-    <t>Equipo desarrollo</t>
-  </si>
-  <si>
     <t>Solicitar informe de pruebas de portabilidad realizados en etapas anteriores del proyecto</t>
   </si>
   <si>
@@ -372,10 +351,6 @@
     <t>Se recomienda la implementación de un sistema de seguimiento de pedidos que permita a los clientes rastrear el estado de sus pedidos y recibir actualizaciones en tiempo real</t>
   </si>
   <si>
-    <t>PO
-Scrum Master</t>
-  </si>
-  <si>
     <t>Se recomienda incorporar pruebas de usabilidad en otras etapas del proyecto para validar que la página web sea fácil de usar y navegar, y que el proceso de compra sea intuitivo para el cliente</t>
   </si>
   <si>
@@ -415,9 +390,6 @@
     <t xml:space="preserve">Utilizar técnica basada en expertos para estimar el esfuerzo de la prueba, basándose en la experiencia de los expertos </t>
   </si>
   <si>
-    <t>Líder técnico</t>
-  </si>
-  <si>
     <t>Cambios en el mercado, de tecnología o políticas que puedan afectar el desarrollo del proyecto</t>
   </si>
   <si>
@@ -434,6 +406,12 @@
   </si>
   <si>
     <t>Posibilidad de recibir respuestas erroneas de los servicios SOAP cuando el usuario ingresa datos de entrada invalidos</t>
+  </si>
+  <si>
+    <t>Diseñar y priorizar los casos de prueba donde se detecten la posibilidad de que el usuario reciba respuetas erroneas</t>
+  </si>
+  <si>
+    <t>Diseñar y priorizar los casos de prueba donde se detecte la posibilidad de que el usuario reciba respuetas erroneas</t>
   </si>
 </sst>
 </file>
@@ -692,6 +670,48 @@
   <dxfs count="56">
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF92D050"/>
       </font>
       <fill>
@@ -905,47 +925,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1431,10 +1410,10 @@
     <tableColumn id="7" xr3:uid="{C40EBB4C-64E3-4329-ACC5-BB89D2E27445}" name="Riesgo" dataDxfId="22"/>
     <tableColumn id="8" xr3:uid="{4F119BEE-18FA-47FA-88FB-21ED334053FD}" name="Riesgo " dataDxfId="21"/>
     <tableColumn id="9" xr3:uid="{3FDDB74E-AF6B-4B35-81C7-640CD8656687}" name="Acción" dataDxfId="20"/>
-    <tableColumn id="10" xr3:uid="{7DA0AD36-AACB-49C6-97E7-9F41DC268BA1}" name="Plan de Acción" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{10D58CD4-A65C-4CE8-87A7-FA74ABFF1C93}" name="Responsable de la Acción" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{FD926A79-4873-4A99-89A9-E351E2B78025}" name="Fecha Compromiso " dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{F55FD157-6FFF-497B-8F3D-C4A8F1183083}" name="Estado" dataDxfId="16"/>
+    <tableColumn id="10" xr3:uid="{7DA0AD36-AACB-49C6-97E7-9F41DC268BA1}" name="Plan de Acción" dataDxfId="2"/>
+    <tableColumn id="11" xr3:uid="{10D58CD4-A65C-4CE8-87A7-FA74ABFF1C93}" name="Responsable de la Acción" dataDxfId="0"/>
+    <tableColumn id="12" xr3:uid="{FD926A79-4873-4A99-89A9-E351E2B78025}" name="Fecha Compromiso " dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{F55FD157-6FFF-497B-8F3D-C4A8F1183083}" name="Estado" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="Matriz de Riesgo-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1443,8 +1422,8 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0F99F682-9124-4141-9886-84FF3DF70E95}" name="Table_2" displayName="Table_2" ref="A1:B5">
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6FCFD6CF-D05E-47EA-A6EC-3BAF9E14DCAE}" name="Plan de Acción" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{78FB452F-ECA1-475A-8C9B-B9544E7D6DDC}" name="Descripción" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{6FCFD6CF-D05E-47EA-A6EC-3BAF9E14DCAE}" name="Plan de Acción" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{78FB452F-ECA1-475A-8C9B-B9544E7D6DDC}" name="Descripción" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1453,7 +1432,7 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5B45C15-A36D-4BC0-9E74-AFD731CE3381}" name="Table_3" displayName="Table_3" ref="D1:D3">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{C85C2E5D-B09A-4D5F-97C0-AB5A81FEEB2A}" name="Tipo de Riesg" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{C85C2E5D-B09A-4D5F-97C0-AB5A81FEEB2A}" name="Tipo de Riesg" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 2" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1462,9 +1441,9 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{7C4D1B14-5B86-4DBF-94FE-8B73D66225C7}" name="Table_4" displayName="Table_4" ref="F1:H6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{CEC6DF00-0D9C-4327-B944-A9256E007FF6}" name="Probabilidad" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{4BF8DB27-E23F-4A92-A495-BB5C0F6632A5}" name="Evaluación" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{21A83028-31E0-46BC-BB5A-34C6ECAFEDD3}" name="Definición" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{CEC6DF00-0D9C-4327-B944-A9256E007FF6}" name="Probabilidad" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4BF8DB27-E23F-4A92-A495-BB5C0F6632A5}" name="Evaluación" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{21A83028-31E0-46BC-BB5A-34C6ECAFEDD3}" name="Definición" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 3" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1473,9 +1452,9 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FDE817A5-0B61-430E-9F87-9AF8174F3EF9}" name="Table_5" displayName="Table_5" ref="J1:L6">
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{63F79449-20E3-4F6D-B5D3-4F3DF0AB1417}" name="Impacto" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{351FFBC1-5848-4E2F-A294-8C5D1675AFA7}" name="Evaluación" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{9BC32A01-D298-4AC4-A8E3-59607DC50617}" name="Definición" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{63F79449-20E3-4F6D-B5D3-4F3DF0AB1417}" name="Impacto" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{351FFBC1-5848-4E2F-A294-8C5D1675AFA7}" name="Evaluación" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{9BC32A01-D298-4AC4-A8E3-59607DC50617}" name="Definición" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 4" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1484,7 +1463,7 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{E9C38933-B1EC-4CE4-82B2-485B6835F881}" name="Table_6" displayName="Table_6" ref="A8:A10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{A4F5C3B6-7FFF-4B5A-AD9D-721C7A161134}" name="Responsable Calidad" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{A4F5C3B6-7FFF-4B5A-AD9D-721C7A161134}" name="Responsable Calidad" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 5" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1493,7 +1472,7 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{27D1D1C5-CBC3-454D-9B03-68A1FB92038C}" name="Table_7" displayName="Table_7" ref="D8:D10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{61089E2C-4840-4002-A9EA-E876FAFC254E}" name="Plan de Calidad" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{61089E2C-4840-4002-A9EA-E876FAFC254E}" name="Plan de Calidad" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 6" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1502,7 +1481,7 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{8E9CFF31-25F5-4F31-8D7A-71C8788590E5}" name="Table_8" displayName="Table_8" ref="F8:F10">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{718A55F6-D7C9-4551-AF65-357BA4E12B01}" name="Historia de Usuario" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{718A55F6-D7C9-4551-AF65-357BA4E12B01}" name="Historia de Usuario" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 7" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1511,7 +1490,7 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1D77D549-EA02-4FB7-B0E5-946DBD6CA201}" name="Table_9" displayName="Table_9" ref="A12:A14">
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{B6AE7DE1-B7F0-4FA4-939E-3F45CBF4E99A}" name="Estado" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B6AE7DE1-B7F0-4FA4-939E-3F45CBF4E99A}" name="Estado" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="Tabla-style 8" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1816,8 +1795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E7AC659-34BE-478B-80F3-AAD59B518E91}">
   <dimension ref="A1:L1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="C37" workbookViewId="0">
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1990,14 +1969,9 @@
       <c r="I8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>95</v>
-      </c>
+      <c r="J8" s="19"/>
       <c r="K8" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="96.75" customHeight="1">
@@ -2025,16 +1999,11 @@
         <v>18</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>112</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>87</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="J9" s="24"/>
       <c r="K9" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="52.5" customHeight="1">
@@ -2062,16 +2031,11 @@
         <v>13</v>
       </c>
       <c r="I10" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>89</v>
-      </c>
+        <v>87</v>
+      </c>
+      <c r="J10" s="19"/>
       <c r="K10" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="59.25" customHeight="1">
@@ -2099,16 +2063,11 @@
         <v>18</v>
       </c>
       <c r="I11" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>87</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="J11" s="24"/>
       <c r="K11" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="33.75" customHeight="1">
@@ -2116,7 +2075,7 @@
         <v>5</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>17</v>
@@ -2136,16 +2095,11 @@
         <v>18</v>
       </c>
       <c r="I12" s="18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>87</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="J12" s="24"/>
       <c r="K12" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45">
@@ -2173,16 +2127,11 @@
         <v>13</v>
       </c>
       <c r="I13" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>93</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="J13" s="24"/>
       <c r="K13" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L13" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="73.5" customHeight="1">
@@ -2210,16 +2159,11 @@
         <v>18</v>
       </c>
       <c r="I14" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="J14" s="19" t="s">
-        <v>95</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="J14" s="19"/>
       <c r="K14" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="93.75" customHeight="1">
@@ -2227,7 +2171,7 @@
         <v>8</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>17</v>
@@ -2247,16 +2191,11 @@
         <v>13</v>
       </c>
       <c r="I15" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>97</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="J15" s="24"/>
       <c r="K15" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="57" customHeight="1">
@@ -2264,7 +2203,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>17</v>
@@ -2284,19 +2223,14 @@
         <v>18</v>
       </c>
       <c r="I16" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="J16" s="19" t="s">
-        <v>99</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="J16" s="19"/>
       <c r="K16" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="63.75" customHeight="1">
+    </row>
+    <row r="17" spans="1:11" ht="63.75" customHeight="1">
       <c r="A17" s="5">
         <v>10</v>
       </c>
@@ -2321,19 +2255,14 @@
         <v>18</v>
       </c>
       <c r="I17" s="18" t="s">
-        <v>100</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>87</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="J17" s="24"/>
       <c r="K17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="45" customHeight="1">
+    </row>
+    <row r="18" spans="1:11" ht="45" customHeight="1">
       <c r="A18" s="5">
         <v>11</v>
       </c>
@@ -2358,19 +2287,14 @@
         <v>18</v>
       </c>
       <c r="I18" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>87</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J18" s="24"/>
       <c r="K18" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L18" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="30">
+    </row>
+    <row r="19" spans="1:11" ht="30">
       <c r="A19" s="5">
         <v>12</v>
       </c>
@@ -2395,19 +2319,14 @@
         <v>13</v>
       </c>
       <c r="I19" s="18" t="s">
-        <v>102</v>
-      </c>
-      <c r="J19" s="19" t="s">
-        <v>99</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="J19" s="19"/>
       <c r="K19" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="54" customHeight="1">
+    </row>
+    <row r="20" spans="1:11" ht="54" customHeight="1">
       <c r="A20" s="5">
         <v>13</v>
       </c>
@@ -2432,24 +2351,19 @@
         <v>13</v>
       </c>
       <c r="I20" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="J20" s="19" t="s">
-        <v>89</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="J20" s="19"/>
       <c r="K20" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="69.75" customHeight="1">
+    </row>
+    <row r="21" spans="1:11" ht="69.75" customHeight="1">
       <c r="A21" s="5">
         <v>14</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>17</v>
@@ -2469,19 +2383,14 @@
         <v>13</v>
       </c>
       <c r="I21" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="J21" s="19" t="s">
-        <v>89</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="J21" s="19"/>
       <c r="K21" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="30">
+    </row>
+    <row r="22" spans="1:11" ht="30">
       <c r="A22" s="5">
         <v>15</v>
       </c>
@@ -2506,19 +2415,14 @@
         <v>18</v>
       </c>
       <c r="I22" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>87</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="J22" s="24"/>
       <c r="K22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L22" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="45">
+    </row>
+    <row r="23" spans="1:11" ht="45">
       <c r="A23" s="5">
         <v>16</v>
       </c>
@@ -2543,24 +2447,19 @@
         <v>18</v>
       </c>
       <c r="I23" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>89</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="J23" s="19"/>
       <c r="K23" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L23" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="42" customHeight="1">
+    </row>
+    <row r="24" spans="1:11" ht="42" customHeight="1">
       <c r="A24" s="5">
         <v>17</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>12</v>
@@ -2580,19 +2479,14 @@
         <v>13</v>
       </c>
       <c r="I24" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>89</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="J24" s="24"/>
       <c r="K24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L24" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="45">
+    </row>
+    <row r="25" spans="1:11" ht="45">
       <c r="A25" s="5">
         <v>18</v>
       </c>
@@ -2617,24 +2511,19 @@
         <v>13</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>95</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="J25" s="19"/>
       <c r="K25" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L25" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="51" customHeight="1">
+    </row>
+    <row r="26" spans="1:11" ht="51" customHeight="1">
       <c r="A26" s="5">
         <v>19</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>12</v>
@@ -2654,19 +2543,14 @@
         <v>13</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="J26" s="19" t="s">
-        <v>95</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="J26" s="19"/>
       <c r="K26" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L26" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="61.5" customHeight="1">
+    </row>
+    <row r="27" spans="1:11" ht="61.5" customHeight="1">
       <c r="A27" s="5">
         <v>20</v>
       </c>
@@ -2691,19 +2575,14 @@
         <v>13</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="J27" s="19" t="s">
-        <v>89</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="J27" s="19"/>
       <c r="K27" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="44.25" customHeight="1">
+    </row>
+    <row r="28" spans="1:11" ht="44.25" customHeight="1">
       <c r="A28" s="5">
         <v>21</v>
       </c>
@@ -2728,19 +2607,14 @@
         <v>18</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="J28" s="19" t="s">
-        <v>89</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="J28" s="19"/>
       <c r="K28" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L28" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="45">
+    </row>
+    <row r="29" spans="1:11" ht="45">
       <c r="A29" s="5">
         <v>22</v>
       </c>
@@ -2765,19 +2639,14 @@
         <v>13</v>
       </c>
       <c r="I29" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="J29" s="19" t="s">
-        <v>95</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="J29" s="19"/>
       <c r="K29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L29" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="60">
+    </row>
+    <row r="30" spans="1:11" ht="60">
       <c r="A30" s="5">
         <v>23</v>
       </c>
@@ -2802,19 +2671,14 @@
         <v>13</v>
       </c>
       <c r="I30" s="25" t="s">
-        <v>123</v>
-      </c>
-      <c r="J30" s="26" t="s">
-        <v>89</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="J30" s="26"/>
       <c r="K30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L30" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" ht="30">
+    </row>
+    <row r="31" spans="1:11" ht="30">
       <c r="A31" s="5">
         <v>24</v>
       </c>
@@ -2839,24 +2703,19 @@
         <v>13</v>
       </c>
       <c r="I31" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="J31" s="26" t="s">
-        <v>125</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="J31" s="26"/>
       <c r="K31" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L31" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="30">
+    </row>
+    <row r="32" spans="1:11" ht="30">
       <c r="A32" s="5">
         <v>25</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>12</v>
@@ -2876,19 +2735,14 @@
         <v>18</v>
       </c>
       <c r="I32" s="25" t="s">
-        <v>127</v>
-      </c>
-      <c r="J32" s="27" t="s">
-        <v>111</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="J32" s="27"/>
       <c r="K32" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="45">
+    </row>
+    <row r="33" spans="1:11" ht="45">
       <c r="A33" s="5">
         <v>26</v>
       </c>
@@ -2913,19 +2767,14 @@
         <v>18</v>
       </c>
       <c r="I33" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="J33" s="26" t="s">
-        <v>95</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="J33" s="26"/>
       <c r="K33" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" ht="30">
+    </row>
+    <row r="34" spans="1:11" ht="30">
       <c r="A34" s="5">
         <v>27</v>
       </c>
@@ -2950,19 +2799,14 @@
         <v>13</v>
       </c>
       <c r="I34" s="25" t="s">
-        <v>106</v>
-      </c>
-      <c r="J34" s="26" t="s">
-        <v>125</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="J34" s="26"/>
       <c r="K34" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L34" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="30">
+    </row>
+    <row r="35" spans="1:11" ht="30">
       <c r="A35" s="5">
         <v>28</v>
       </c>
@@ -2987,19 +2831,14 @@
         <v>13</v>
       </c>
       <c r="I35" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="J35" s="26" t="s">
-        <v>89</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="J35" s="26"/>
       <c r="K35" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L35" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" ht="30">
+    </row>
+    <row r="36" spans="1:11" ht="30">
       <c r="A36" s="5">
         <v>29</v>
       </c>
@@ -3024,19 +2863,14 @@
         <v>13</v>
       </c>
       <c r="I36" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="J36" s="26" t="s">
-        <v>89</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="J36" s="26"/>
       <c r="K36" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="45">
+    </row>
+    <row r="37" spans="1:11" ht="45">
       <c r="A37" s="5">
         <v>30</v>
       </c>
@@ -3061,24 +2895,19 @@
         <v>18</v>
       </c>
       <c r="I37" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="J37" s="26" t="s">
-        <v>99</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="J37" s="26"/>
       <c r="K37" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="L37" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" ht="30">
+    </row>
+    <row r="38" spans="1:11" ht="30">
       <c r="A38" s="8">
         <v>31</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>17</v>
@@ -3097,15 +2926,20 @@
       <c r="H38" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="28"/>
-    </row>
-    <row r="39" spans="1:12" ht="30">
+      <c r="I38" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="J38" s="8"/>
+      <c r="K38" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30">
       <c r="A39" s="33">
         <v>32</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>17</v>
@@ -3124,42 +2958,47 @@
       <c r="H39" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="10"/>
-      <c r="J39" s="28"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1">
+      <c r="I39" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J39" s="8"/>
+      <c r="K39" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="I40" s="6"/>
     </row>
-    <row r="41" spans="1:12" ht="15.75" customHeight="1">
+    <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="1:12" ht="15.75" customHeight="1">
+    <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="I42" s="6"/>
     </row>
-    <row r="43" spans="1:12" ht="15.75" customHeight="1">
+    <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="I43" s="6"/>
     </row>
-    <row r="44" spans="1:12" ht="15.75" customHeight="1">
+    <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="I44" s="6"/>
     </row>
-    <row r="45" spans="1:12" ht="15.75" customHeight="1">
+    <row r="45" spans="1:11" ht="15.75" customHeight="1">
       <c r="I45" s="6"/>
     </row>
-    <row r="46" spans="1:12" ht="15.75" customHeight="1" thickBot="1">
+    <row r="46" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="B46" s="31" t="s">
         <v>20</v>
       </c>
       <c r="C46" s="32"/>
       <c r="I46" s="6"/>
     </row>
-    <row r="47" spans="1:12" ht="15.75" customHeight="1">
+    <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="B47" s="12" t="s">
         <v>21</v>
       </c>
       <c r="C47" s="13"/>
       <c r="I47" s="6"/>
     </row>
-    <row r="48" spans="1:12" ht="15.75" customHeight="1">
+    <row r="48" spans="1:11" ht="15.75" customHeight="1">
       <c r="B48" s="14" t="s">
         <v>22</v>
       </c>
@@ -6059,15 +5898,15 @@
     <mergeCell ref="B46:C46"/>
   </mergeCells>
   <conditionalFormatting sqref="G8:G1009">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
       <formula>20</formula>
       <formula>25</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
       <formula>11</formula>
       <formula>19</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="between">
       <formula>1</formula>
       <formula>10</formula>
     </cfRule>

</xml_diff>